<commit_message>
Testing again for hexbin
</commit_message>
<xml_diff>
--- a/data/information/gp_list.xlsx
+++ b/data/information/gp_list.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wh0102/Downloads/github/mph/geo_project/data/gp/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wh0102/Downloads/github/mph_research/data/information/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD06E89A-FA1F-7E45-BF2D-A2523579958F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10E31E56-5540-2044-9952-DBE425277F49}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15820" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
   </definedNames>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="4" r:id="rId3"/>
+    <pivotCache cacheId="0" r:id="rId3"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -19811,7 +19811,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{D5B08F05-3DF3-0147-ADC1-EA89BD3735A2}" name="PivotTable1" cacheId="4" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="17">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{D5B08F05-3DF3-0147-ADC1-EA89BD3735A2}" name="PivotTable1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="17">
   <location ref="A3:B21" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="7">
     <pivotField axis="axisRow" showAll="0" sortType="ascending">
@@ -20652,7 +20652,9 @@
   </sheetPr>
   <dimension ref="A1:H1258"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A545" workbookViewId="0">
+      <selection activeCell="H572" sqref="H572"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
@@ -35370,10 +35372,10 @@
         <v>101.40756</v>
       </c>
       <c r="G566" s="1" t="s">
-        <v>2221</v>
+        <v>2223</v>
       </c>
       <c r="H566" t="s">
-        <v>2220</v>
+        <v>2222</v>
       </c>
     </row>
     <row r="567" spans="1:8" ht="13" x14ac:dyDescent="0.15">
@@ -45608,10 +45610,10 @@
         <v>1675</v>
       </c>
       <c r="E960" s="2">
-        <v>31.406363200000001</v>
+        <v>6.0000254928024601</v>
       </c>
       <c r="F960" s="2">
-        <v>73.106929800000003</v>
+        <v>116.129212005616</v>
       </c>
       <c r="G960" s="2" t="s">
         <v>2211</v>
@@ -46960,10 +46962,10 @@
         <v>1773</v>
       </c>
       <c r="E1012" s="2">
-        <v>3.5951955999999998</v>
+        <v>4.5558788426654298</v>
       </c>
       <c r="F1012" s="2">
-        <v>98.672222700000006</v>
+        <v>101.114148872698</v>
       </c>
       <c r="G1012" s="2" t="s">
         <v>2210</v>

</xml_diff>